<commit_message>
Update evidence for task A7-A20
</commit_message>
<xml_diff>
--- a/ben-razor/evidence.xlsx
+++ b/ben-razor/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -160,19 +160,157 @@
     <t xml:space="preserve">gon-flixnet-1 </t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on that chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on that chain	chain id</t>
+    <t xml:space="preserve">ibc/3101428715B27054F89013DAEAAEE228B2F49AA545401AF2DAAF88640C9263A6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/A713B02A768CAD2F7FE302B7943AF42763A7A74DCEB07A7A544DEDFE599C0E34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/CA5730BEA8CCD9C9BC6A00ED7EFCFFB1FA596F04C5FA9ECC9DFC8B2BFF47356A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/73184169EEF7A193FF185E572969EE521BB77263343A69810F4A902FE7B54255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/66C5554D7331FA925539B80EC49F611EB92C4E9FF82DE877E75A3F5A53D793C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/67B9F02FA0AEA21EFDD35CD080F33AF7CC0B1232F3FCA56C0A0F5D60B659BCDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2070897CA2BB9443D1519E2D42475E326260A12D235F77EC7F6683EFEFC10D47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-irishub-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475155FE3F4AF328CD734B01614B90B635C7E13760F8217C98843800A72BD3D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42E17A1C103D405DCAD02AD8536849A1E580121F81CC9F5775676EDF59CCB7F7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uptick_7000-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D519D83C9F50915E10FD2FF9303633F0974A7B986979B1F324A174F0CAADEF70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320A032F52632E280C6A57FED33060C35A17482D16A834A5CECE4B6487EBDF54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14FD598B3EFC58917E25DBD53DED7538E7A11BBDB4FCEDBC5B6020E06A3FBCD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9F996238905D410D0D2665213DBF048508C77F2E549F2343D4AA3C3E1407E9B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">887FC883D6DE79033C87F9BC2ECDE05042279FF097F7E086EFFA06EE3AE8EE59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31356DA544191232ABDBCEA7A74C077F32F017A9EB091C8BC2046CE83951C85B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2C6464993D9CB79DF78F8601A61DFFB22EB08603F7B0DF0C0076B75A1E955C60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9380BD294B4345C94ACF7E5C66B2C3F435741622DBF1CE3912455D1B3252E985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80666B729A09DC95B90281A35E7B3910D9446DD3A54069F197CAD79163ABF559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603234A289F21D5F7D5584B5321739BD20B19A28228A569FE187B179E18AF463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">843F38026063156AA31D076E44C037D579275F5AB6C4BAE171F36AC0198C175D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B9D6C4059AF8B8D33B9CC5F7047FA46630EB1EADA71DA9D1093322CA49006E54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01F3C31C45AB790679CE33F7DC70CF09EDDCD0E001ECC2B632D94FB0DD95266B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3F650E80A10587C0E6F0147CFC414C8709B8B4173486A7CF024C72B1AA069FC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F010211EDA76682D7452CF03D6CB53A6BCBE266CFA42171D9EC6AD69A03A7EDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">588D51CBF835B33CD5C65D3E105248C6B6CF7AB924BFA7CE9C276A43D57F809C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F096609C9242149C16736F5C124E190D6E4E7E4E490EFDC2CEEAC217C309D96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21AF648758E1426D8CE29C054596DB47F32A47D9B8BA8FFE777CECFC9F387E7D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54E7DB9BB035049C3C4BB0BE9DDF965603D96CD326B6D9F2C7BE055D1A722642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31AC694B24FDCE78EC1CBDBEE8391E84A8D17BE1977BE837E3D8129FA56731DD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">786C90750AB9E96CCA13B906C7B88D05FB742892687E1D87DCDDA8B436CFD210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA2CBD88C4E625200F689C621747A86B15C184424F83FC0DBFAAFA90D7A68B2D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68FEB8C1790201EAC480547F527FC029AAA8423BD89B057C651C3B89414EB177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56A1A4A13FF34CB10BEA39C61EB0B9A11EE2E62CD8557CBE286A946389D17FDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">960138411D65C59BBF9A01DAEB8D533B6D5A53FE7CCE6C36894D5D11ECEE3435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0BD753D31014D7CA3C6EA7F3E150F61C9EC348645E9A674B1AD3C42459A961D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8312A8DA646816474BEFD198F4296911F3A170DFA4F8E5F4787C7606D1A9988B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCCC0683D620555303B32399EA6A93F7C2BB6D7007B12A27F8F585CA72F24143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F26F6C0CCB0FD03E0033F498983CC8AA026540C06CD02F8F1D605EC03E7C4EFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3BD62245B22B7F6551FACE5741D829E11074D2F0C0BF04F7A255AFCD145EE3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">660D2461E2323E139EAA2B2C0D90158C0665A95E6F72D03FA2684A41177915A9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66800B06540A82BECB850E45F94E1D67FE69C8A7CA554826F9920BA5E82D8B2E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2EF7ED8B5640F5320B6B6E62AA628B1D08C7110A3E489318F0FAA5E9D75BD9AE</t>
   </si>
   <si>
     <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
@@ -188,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -217,6 +355,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -288,7 +432,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,6 +455,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -393,7 +545,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,7 +631,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -498,10 +650,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -523,7 +675,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,10 +694,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -567,7 +719,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -586,10 +738,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -611,7 +763,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -630,10 +782,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -652,10 +804,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -674,20 +826,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -706,10 +872,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -728,20 +894,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>57</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>58</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -760,10 +940,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -782,20 +962,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>61</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>63</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -814,10 +1008,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -836,20 +1030,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>66</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -868,10 +1076,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -890,20 +1098,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>70</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>71</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -922,10 +1144,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,20 +1166,34 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>74</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>75</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -978,7 +1214,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1019,10 +1255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1041,20 +1277,50 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>78</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>79</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1073,10 +1339,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1095,20 +1361,50 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>84</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>85</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1145,12 +1441,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1187,12 +1483,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1229,12 +1525,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1271,12 +1567,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1529,7 +1825,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1588,7 +1884,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1632,7 +1928,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1651,10 +1947,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update evidence for task B1-B4
</commit_message>
<xml_diff>
--- a/ben-razor/evidence.xlsx
+++ b/ben-razor/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -311,6 +311,18 @@
   </si>
   <si>
     <t xml:space="preserve">2EF7ED8B5640F5320B6B6E62AA628B1D08C7110A3E489318F0FAA5E9D75BD9AE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E8750EF477359BFC9C9E6271E1DE16ECFF0D1AC4DE27B5D649C586AF0FCB32D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03E4D08C44032891A8577581B10D5899CADD768B4C8D6BD1606AD76CE9032005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6FC5A35A43506803589761F04554EDF5009C4F4FED438FB782CB7899EC23F50C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">643454247835F2A7F7CE4F251E55C009B150A220836D8A733A7AE96B47FFE416</t>
   </si>
   <si>
     <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
@@ -326,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -355,12 +367,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -432,7 +438,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -458,10 +464,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1176,7 +1178,7 @@
       <c r="A3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1192,7 +1194,7 @@
       <c r="A5" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1426,7 +1428,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1467,8 +1469,8 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1483,12 +1485,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1525,12 +1527,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1567,12 +1569,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1827,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update evidence for task B5-B7
</commit_message>
<xml_diff>
--- a/ben-razor/evidence.xlsx
+++ b/ben-razor/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
     <sheet name="B2" sheetId="23" state="visible" r:id="rId24"/>
     <sheet name="B5" sheetId="24" state="visible" r:id="rId25"/>
     <sheet name="B6" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="B7" sheetId="26" state="visible" r:id="rId27"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="99">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -325,10 +326,22 @@
     <t xml:space="preserve">643454247835F2A7F7CE4F251E55C009B150A220836D8A733A7AE96B47FFE416</t>
   </si>
   <si>
-    <t xml:space="preserve">The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Internal Transfer TxHash on IRISnet</t>
+    <t xml:space="preserve">38EF6D816E6023D81C3C18B7A5AB13C4AF90672FBB24A71FB84C866F839CD5B7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">559B4D3C0168B6604706DA75DD04A5A65A0A1F5151B6FD8B6E1CE7ADF835B6FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E7AA928546213422290DB7A141A2EEB3D7CA80D9F291865CFA3B77D823FCEAFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47A6FDDD23F2E47095193ACD964DADA94FD0B6EC2E4B29A21A3D6E70DEF83BA5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD7A8876EA276D3D3279D63F8FB0A53B15E5639B9F2471BC9802A0F7B6313EED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E6C6C2E27F6EB9990A1855CF60376ED95B2AF6B1D08841BAF0FF92CA80815FD9</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1482,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1512,7 +1525,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1554,7 +1567,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,12 +1582,54 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>